<commit_message>
Agrega primera iteracion de posicion
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="83">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posicion</t>
   </si>
   <si>
     <t xml:space="preserve">Es Base</t>
@@ -362,16 +365,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G72" activeCellId="0" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,21 +403,27 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -419,21 +432,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -442,21 +458,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -465,21 +484,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -488,21 +510,24 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -511,21 +536,24 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -534,21 +562,24 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>6</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -557,21 +588,24 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>6</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -580,21 +614,24 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -603,21 +640,24 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>6</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -626,21 +666,24 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -649,21 +692,24 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -672,21 +718,24 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>6</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -695,21 +744,24 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>13</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -718,21 +770,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>13</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -741,21 +796,24 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>13</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -764,15 +822,18 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -781,21 +842,24 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -804,21 +868,24 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -827,21 +894,24 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -850,21 +920,24 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -873,21 +946,24 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>21</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -896,21 +972,24 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>21</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -919,21 +998,24 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>21</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -942,21 +1024,24 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -965,21 +1050,24 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>25</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -988,21 +1076,24 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>25</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1011,21 +1102,24 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1034,21 +1128,24 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1057,21 +1154,24 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1080,21 +1180,24 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1103,21 +1206,24 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1126,21 +1232,24 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1149,21 +1258,24 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1172,21 +1284,24 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1195,21 +1310,24 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1218,21 +1336,24 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1241,21 +1362,24 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1264,21 +1388,24 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1287,21 +1414,24 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>39</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1310,21 +1440,24 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>39</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1333,21 +1466,24 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1356,21 +1492,24 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>42</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1379,21 +1518,24 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>42</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1402,15 +1544,18 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1419,21 +1564,24 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>45</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1442,21 +1590,24 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>45</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1465,21 +1616,24 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>45</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1488,21 +1642,24 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>45</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1511,21 +1668,24 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>45</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1534,21 +1694,24 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>50</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1557,21 +1720,24 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>50</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1580,21 +1746,24 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>50</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1603,21 +1772,24 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>50</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1626,15 +1798,18 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1643,21 +1818,24 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>55</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1666,21 +1844,24 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>56</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1689,21 +1870,24 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>56</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1712,21 +1896,24 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>55</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1735,21 +1922,24 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>55</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1758,21 +1948,24 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>55</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1781,21 +1974,24 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>68</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>61</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1804,21 +2000,24 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>61</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1827,21 +2026,24 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>61</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1850,21 +2052,24 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>61</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1873,15 +2078,18 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1890,21 +2098,24 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>66</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1913,21 +2124,24 @@
         <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>66</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1936,21 +2150,24 @@
         <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>68</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1959,21 +2176,24 @@
         <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>68</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1982,21 +2202,24 @@
         <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>68</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2005,21 +2228,24 @@
         <v>72</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>68</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2028,21 +2254,24 @@
         <v>73</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>68</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2051,21 +2280,24 @@
         <v>74</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>68</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modifica ID nodos para arrancar desde 0
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="84">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve">Agropecuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pérdidas por Transformación</t>
   </si>
 </sst>
 </file>
@@ -365,10 +368,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G72" activeCellId="0" sqref="G72"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -409,7 +412,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>8</v>
@@ -429,7 +432,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -455,7 +458,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>10</v>
@@ -481,7 +484,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>11</v>
@@ -507,7 +510,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>12</v>
@@ -533,7 +536,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>13</v>
@@ -559,7 +562,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>14</v>
@@ -585,7 +588,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>15</v>
@@ -611,7 +614,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>16</v>
@@ -637,7 +640,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>17</v>
@@ -663,7 +666,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>18</v>
@@ -689,7 +692,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>19</v>
@@ -715,7 +718,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>20</v>
@@ -741,7 +744,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>21</v>
@@ -767,7 +770,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>22</v>
@@ -793,7 +796,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>23</v>
@@ -819,7 +822,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>24</v>
@@ -839,7 +842,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>25</v>
@@ -865,7 +868,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>26</v>
@@ -891,7 +894,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>27</v>
@@ -917,7 +920,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>28</v>
@@ -943,7 +946,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>29</v>
@@ -969,7 +972,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>30</v>
@@ -995,7 +998,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>31</v>
@@ -1021,7 +1024,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>32</v>
@@ -1047,7 +1050,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>33</v>
@@ -1073,7 +1076,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>34</v>
@@ -1099,7 +1102,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>35</v>
@@ -1125,7 +1128,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>36</v>
@@ -1151,7 +1154,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>37</v>
@@ -1177,7 +1180,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>38</v>
@@ -1203,7 +1206,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>39</v>
@@ -1229,7 +1232,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>40</v>
@@ -1255,7 +1258,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>41</v>
@@ -1281,7 +1284,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>42</v>
@@ -1307,7 +1310,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>43</v>
@@ -1333,7 +1336,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>44</v>
@@ -1359,7 +1362,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>45</v>
@@ -1385,7 +1388,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>46</v>
@@ -1411,7 +1414,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>47</v>
@@ -1437,7 +1440,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>48</v>
@@ -1463,7 +1466,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>49</v>
@@ -1489,7 +1492,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>50</v>
@@ -1515,7 +1518,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>51</v>
@@ -1541,7 +1544,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>52</v>
@@ -1561,7 +1564,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>53</v>
@@ -1587,7 +1590,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>54</v>
@@ -1613,7 +1616,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>55</v>
@@ -1639,7 +1642,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>56</v>
@@ -1665,7 +1668,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>57</v>
@@ -1691,7 +1694,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>58</v>
@@ -1717,7 +1720,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>60</v>
@@ -1743,7 +1746,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>61</v>
@@ -1769,7 +1772,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>62</v>
@@ -1795,7 +1798,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>63</v>
@@ -1815,7 +1818,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>64</v>
@@ -1841,7 +1844,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>65</v>
@@ -1867,7 +1870,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>66</v>
@@ -1893,7 +1896,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>67</v>
@@ -1919,7 +1922,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>68</v>
@@ -1945,7 +1948,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>69</v>
@@ -1971,7 +1974,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>70</v>
@@ -1997,7 +2000,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>71</v>
@@ -2023,7 +2026,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>72</v>
@@ -2049,7 +2052,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>73</v>
@@ -2075,7 +2078,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>74</v>
@@ -2095,7 +2098,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>75</v>
@@ -2121,7 +2124,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>76</v>
@@ -2147,7 +2150,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>77</v>
@@ -2173,7 +2176,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>78</v>
@@ -2199,7 +2202,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>79</v>
@@ -2225,7 +2228,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>80</v>
@@ -2251,7 +2254,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>81</v>
@@ -2277,7 +2280,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>82</v>
@@ -2299,6 +2302,26 @@
       </c>
       <c r="H75" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrega nodos 'de relleno' al maestro de nodos; agrega cálculo de posicionY dentro de generar_datos_anio
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -20,15 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Posicion</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posicionX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posicionY</t>
   </si>
   <si>
     <t xml:space="preserve">Energía Hidráulica</t>
@@ -155,6 +158,12 @@
   </si>
   <si>
     <t xml:space="preserve">Gasolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pérdidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">borrar</t>
   </si>
 </sst>
 </file>
@@ -255,17 +264,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,13 +285,16 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -295,7 +305,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -306,7 +316,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -317,7 +327,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -328,7 +338,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -339,7 +349,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -350,7 +360,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -361,7 +371,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -372,7 +382,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -383,7 +393,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -394,7 +404,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -405,7 +415,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
@@ -416,7 +426,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>5</v>
@@ -427,7 +437,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>3</v>
@@ -438,7 +448,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>3</v>
@@ -449,7 +459,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>3</v>
@@ -460,7 +470,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>3</v>
@@ -471,7 +481,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>3</v>
@@ -482,7 +492,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>3</v>
@@ -493,7 +503,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>3</v>
@@ -504,7 +514,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>3</v>
@@ -515,7 +525,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>3</v>
@@ -526,7 +536,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>3</v>
@@ -537,7 +547,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>3</v>
@@ -548,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>3</v>
@@ -559,7 +569,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>3</v>
@@ -570,7 +580,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>4</v>
@@ -581,7 +591,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>2</v>
@@ -592,7 +602,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>2</v>
@@ -603,7 +613,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>2</v>
@@ -614,10 +624,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,7 +638,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>6</v>
@@ -636,7 +649,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>6</v>
@@ -647,7 +660,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>6</v>
@@ -658,7 +671,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>6</v>
@@ -669,7 +682,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>6</v>
@@ -680,7 +693,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>6</v>
@@ -691,10 +704,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,7 +718,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>3</v>
@@ -713,7 +729,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>3</v>
@@ -724,7 +740,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>3</v>
@@ -735,10 +751,94 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="C43" s="0" t="n">
-        <v>3</v>
+      <c r="B46" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementa cambios del Issue #1: Unificar nodos de Pérdidas y Pérdidas por Transformación
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Agropecuario</t>
   </si>
   <si>
-    <t xml:space="preserve">Pérdidas por Transformación</t>
+    <t xml:space="preserve">Pérdidas</t>
   </si>
   <si>
     <t xml:space="preserve">Coque</t>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gasolina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pérdidas</t>
   </si>
   <si>
     <t xml:space="preserve">borrar</t>
@@ -264,17 +261,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,13 +758,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>46</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>1</v>
@@ -775,72 +772,58 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="C48" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Elimina dos nodos 'borrar' y agrega los nodos Importación y Exportación
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t xml:space="preserve">Gasolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exportación</t>
   </si>
   <si>
     <t xml:space="preserve">borrar</t>
@@ -263,8 +269,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -758,38 +764,32 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>46</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>6</v>
@@ -800,10 +800,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>6</v>
@@ -814,10 +814,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
Modifica agrupamientos energias MINEM para coincidir con las últimas especificaciones
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -88,30 +88,6 @@
     <t xml:space="preserve">Motonaftas</t>
   </si>
   <si>
-    <t xml:space="preserve">Biodiesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioetanol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas de Alto Horno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbón Residual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas de Refinería</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kerosene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otras Naftas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas de Coquería</t>
-  </si>
-  <si>
     <t xml:space="preserve">Centrales Eléctricas</t>
   </si>
   <si>
@@ -148,22 +124,19 @@
     <t xml:space="preserve">Pérdidas</t>
   </si>
   <si>
-    <t xml:space="preserve">Coque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbón de Leña</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Energéticos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gasolina</t>
-  </si>
-  <si>
     <t xml:space="preserve">Importación</t>
   </si>
   <si>
     <t xml:space="preserve">Exportación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biocombustibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otros Gases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras Secundarias</t>
   </si>
   <si>
     <t xml:space="preserve">borrar</t>
@@ -241,12 +214,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,17 +236,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,197 +461,200 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>39</v>
@@ -692,137 +662,35 @@
       <c r="C37" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D48" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Acorto nombres de nodos con demasiados caracteres
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Energía Nuclear</t>
   </si>
   <si>
-    <t xml:space="preserve">Gas Natural de Pozo</t>
+    <t xml:space="preserve">Gas Natural</t>
   </si>
   <si>
     <t xml:space="preserve">Petróleo</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Energía Eléctrica</t>
   </si>
   <si>
-    <t xml:space="preserve">Gas Distribuido por Redes</t>
+    <t xml:space="preserve">Gas de Red</t>
   </si>
   <si>
     <t xml:space="preserve">Gas Licuado</t>
@@ -91,13 +91,13 @@
     <t xml:space="preserve">Centrales Eléctricas</t>
   </si>
   <si>
-    <t xml:space="preserve">Plantas de Tratamiento de Gas</t>
+    <t xml:space="preserve">Plantas de Gas</t>
   </si>
   <si>
     <t xml:space="preserve">Refinerías</t>
   </si>
   <si>
-    <t xml:space="preserve">Otros Centros de Transformación</t>
+    <t xml:space="preserve">Otros Centros</t>
   </si>
   <si>
     <t xml:space="preserve">Consumo Propio</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
-    <t xml:space="preserve">Consumo No Energético</t>
+    <t xml:space="preserve">No Energético</t>
   </si>
   <si>
     <t xml:space="preserve">Transporte</t>
@@ -238,13 +238,15 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Agrega los dos nodos de escala junto con su enlace
</commit_message>
<xml_diff>
--- a/maestro-nodos.xlsx
+++ b/maestro-nodos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t xml:space="preserve">borrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escala1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escala2</t>
   </si>
 </sst>
 </file>
@@ -236,17 +242,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,7 +469,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>22</v>
@@ -474,7 +480,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>23</v>
@@ -485,7 +491,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>24</v>
@@ -496,7 +502,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>25</v>
@@ -507,7 +513,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>26</v>
@@ -521,7 +527,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>27</v>
@@ -532,7 +538,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>28</v>
@@ -543,7 +549,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>29</v>
@@ -554,7 +560,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>30</v>
@@ -565,7 +571,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>31</v>
@@ -576,7 +582,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>32</v>
@@ -587,7 +593,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>33</v>
@@ -601,7 +607,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>34</v>
@@ -612,7 +618,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>35</v>
@@ -623,7 +629,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>36</v>
@@ -634,7 +640,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>37</v>
@@ -645,7 +651,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>38</v>
@@ -656,7 +662,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>39</v>
@@ -670,7 +676,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>39</v>
@@ -684,7 +690,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>39</v>
@@ -693,6 +699,34 @@
         <v>6</v>
       </c>
       <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D41" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>